<commit_message>
Updated script to save funnel plot and output number of studies and sample sizes per outcome.
</commit_message>
<xml_diff>
--- a/output/results_REML_robust.xlsx
+++ b/output/results_REML_robust.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="coefs" sheetId="1" r:id="rId1"/>
     <sheet name="eggers" sheetId="2" r:id="rId2"/>
+    <sheet name="nr_studies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1162,4 +1163,346 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>outcome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>n_effect_sizes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>k_studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MR (tot)</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAIR</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A/FF</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GC/TA</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CCK</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Fun and enjoyment</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ITC</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cognitive skills (PYD)</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Initiative (PYD)</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Negative experiences (PYD)</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Personal and social skills (PYD)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Goal setting (PYD)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MR (amotivation)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MR (controlled)</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MR (self-determined)</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>INSB</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>INTB</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BPNF</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BPNS</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AGT/MC task-related</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Parentsupp</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>